<commit_message>
feat: Dashboard enhancements, QuickContacts integration, and IBAN display
- Enhanced Admin Dashboard with gradient cards and improved UI
- Added IBAN display to user dashboard hero card
- Integrated QuickContacts with real user account IBANs
- Fixed transfer validation and IBAN lookup
- Removed PDF export (unstable), kept CSV export
- Updated pie chart to show real spending categories
- Improved error handling and logging
- Cleaned up temporary files and build artifacts
</commit_message>
<xml_diff>
--- a/Musteriler.xlsx
+++ b/Musteriler.xlsx
@@ -84,7 +84,7 @@
     <t>For evaluation purposes only. Please register an existing license (devexpress.com/DX1000)</t>
   </si>
   <si>
-    <t>or purchase a new license (devexpress.com/BUY) to continue use of DevExpress product libraries (v25.1.7.0).</t>
+    <t>or purchase a new license (devexpress.com/BUY) to continue use of DevExpress product libraries (v25.2.3.0).</t>
   </si>
   <si>
     <t>Included in Subscriptions: Universal, DXperience, WinForms.</t>
@@ -485,7 +485,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>55</v>
+        <v>482</v>
       </c>
       <c t="s" r="B2" s="2">
         <v>10</v>
@@ -509,15 +509,15 @@
         <v>32887.916666666664</v>
       </c>
       <c r="I2" s="1">
-        <v>44</v>
+        <v>252</v>
       </c>
       <c r="J2" s="3">
-        <v>46009.370355262974</v>
+        <v>46025.683620825424</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>56</v>
+        <v>483</v>
       </c>
       <c t="s" r="B3" s="2">
         <v>16</v>
@@ -541,10 +541,10 @@
         <v>31186.875</v>
       </c>
       <c r="I3" s="1">
-        <v>45</v>
+        <v>253</v>
       </c>
       <c r="J3" s="3">
-        <v>46009.370355262974</v>
+        <v>46025.683620825424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>